<commit_message>
hardware: outputs: board_bom: Swaping manually the picoblade vertical component to the right angle version #5
</commit_message>
<xml_diff>
--- a/outputs/board_bom/board_bom.xlsx
+++ b/outputs/board_bom/board_bom.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yan Azeredo\Desktop\SpaceLab\battery-module-4c\outputs\board_bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97045584-F8B2-4413-8E34-804951965D21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364BE09A-2176-4449-BC86-993D9B683BD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
   <si>
     <t>Bill of Materials</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Cylindrical Battery Contacts, Clips, Holders &amp; Springs 16-19mm PC BATTERY CLIP</t>
   </si>
   <si>
-    <t>Headers &amp; Wire Housings VERTICAL HDR SMT 8P</t>
-  </si>
-  <si>
     <t>Connector</t>
   </si>
   <si>
@@ -150,9 +147,6 @@
     <t>Vishay</t>
   </si>
   <si>
-    <t>53398-0871</t>
-  </si>
-  <si>
     <t>67996-110HLF</t>
   </si>
   <si>
@@ -183,9 +177,6 @@
     <t xml:space="preserve"> Cylindrical Contact Clip </t>
   </si>
   <si>
-    <t xml:space="preserve">PicoBlade 53398 </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Through Hole </t>
   </si>
   <si>
@@ -208,6 +199,12 @@
   </si>
   <si>
     <t>Field=bat2_project</t>
+  </si>
+  <si>
+    <t>Connector Header Surface Mount, Right Angle 8 position 0.049" (1.25mm)</t>
+  </si>
+  <si>
+    <t>PicoBlade 53261</t>
   </si>
 </sst>
 </file>
@@ -389,15 +386,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -406,9 +394,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -441,6 +426,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -788,7 +785,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,388 +807,388 @@
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
+      <c r="E2" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="23"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9" t="s">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
+      <c r="E3" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="23"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
+      <c r="E4" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="23"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9" t="s">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
+      <c r="E5" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="23"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="13" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="15" t="s">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="12">
         <f ca="1">TODAY()</f>
-        <v>44103</v>
-      </c>
-      <c r="F7" s="17">
+        <v>44107</v>
+      </c>
+      <c r="F7" s="13">
         <f ca="1">NOW()</f>
-        <v>44103.948272222224</v>
-      </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
+        <v>44107.86014675926</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="G10" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="H10" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="20" t="s">
+      <c r="I10" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="20" t="s">
+      <c r="J10" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="20" t="s">
+      <c r="K10" s="16" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="22">
+      <c r="A11" s="18">
         <f>ROW(A11) - ROW($A$10)</f>
         <v>1</v>
       </c>
-      <c r="B11" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="21">
+      <c r="B11" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="17">
         <v>4</v>
       </c>
-      <c r="D11" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21">
+      <c r="D11" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17">
         <v>32207595</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="I11" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="J11" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="K11" s="21" t="s">
-        <v>32</v>
+      <c r="H11" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="K11" s="17" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="102" x14ac:dyDescent="0.25">
-      <c r="A12" s="22">
+      <c r="A12" s="18">
         <f t="shared" ref="A12:A16" si="0">ROW(A12) - ROW($A$10)</f>
         <v>2</v>
       </c>
-      <c r="B12" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="21">
+      <c r="B12" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="17">
         <v>8</v>
       </c>
-      <c r="D12" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21">
+      <c r="D12" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17">
         <v>54</v>
       </c>
-      <c r="G12" s="21" t="s">
+      <c r="G12" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="I12" s="21">
+      <c r="H12" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" s="17">
         <v>54</v>
       </c>
-      <c r="J12" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="K12" s="21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="22">
+      <c r="J12" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="K12" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="18">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B13" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="21">
+      <c r="B13" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="17">
         <v>2</v>
       </c>
-      <c r="D13" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="I13" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="J13" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="K13" s="21" t="s">
-        <v>32</v>
+      <c r="D13" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17">
+        <v>532610871</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="I13" s="17">
+        <v>532610871</v>
+      </c>
+      <c r="J13" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="K13" s="17" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="22">
+      <c r="A14" s="18">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B14" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="23">
+      <c r="B14" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="19">
         <v>1</v>
       </c>
-      <c r="D14" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="H14" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="I14" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="J14" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K14" s="23" t="s">
-        <v>32</v>
+      <c r="D14" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="K14" s="19" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="22">
+      <c r="A15" s="18">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B15" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="23">
+      <c r="B15" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="19">
         <v>2</v>
       </c>
-      <c r="D15" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="H15" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="I15" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="J15" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K15" s="23" t="s">
-        <v>32</v>
+      <c r="D15" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="I15" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="K15" s="19" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="22">
+      <c r="A16" s="18">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="19">
+        <v>2</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="I16" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="J16" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" s="19" t="s">
         <v>31</v>
-      </c>
-      <c r="C16" s="23">
-        <v>2</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="I16" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="J16" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="K16" s="23" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>